<commit_message>
New Blog post - Race predictons
</commit_message>
<xml_diff>
--- a/blog/posts/RaceTimePrediction/data/tanda.xlsx
+++ b/blog/posts/RaceTimePrediction/data/tanda.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://connectqutedu-my.sharepoint.com/personal/edwardcr_qut_edu_au/Documents/Research/_website/edwchris.github.io/blog/posts/RaceTimePrediction/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{2F08EAEC-4FFA-42EC-94CE-55A5720A8758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A049222-BA87-463F-9E7C-1B30BFB44865}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{2F08EAEC-4FFA-42EC-94CE-55A5720A8758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8448E599-FCCA-4D78-8D07-C53747547E49}"/>
   <bookViews>
-    <workbookView xWindow="5990" yWindow="0" windowWidth="28920" windowHeight="20880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2540" yWindow="70" windowWidth="33170" windowHeight="20880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>Race</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>FinishTime</t>
+  </si>
+  <si>
+    <t>Second</t>
+  </si>
+  <si>
+    <t>P</t>
   </si>
 </sst>
 </file>
@@ -461,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y13"/>
+  <dimension ref="A1:AA13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
+      <selection activeCell="W20" sqref="W20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -482,13 +488,13 @@
     <col min="17" max="17" width="10.81640625" customWidth="1"/>
     <col min="18" max="18" width="13.81640625" customWidth="1"/>
     <col min="19" max="19" width="13" customWidth="1"/>
-    <col min="20" max="20" width="13.08984375" customWidth="1"/>
-    <col min="21" max="22" width="13.1796875" customWidth="1"/>
-    <col min="23" max="23" width="11.26953125" customWidth="1"/>
-    <col min="24" max="24" width="17.54296875" customWidth="1"/>
+    <col min="20" max="20" width="10.36328125" customWidth="1"/>
+    <col min="21" max="24" width="13.1796875" customWidth="1"/>
+    <col min="25" max="25" width="11.26953125" customWidth="1"/>
+    <col min="26" max="26" width="17.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -553,16 +559,22 @@
         <v>31</v>
       </c>
       <c r="V1" t="s">
+        <v>32</v>
+      </c>
+      <c r="W1" t="s">
+        <v>33</v>
+      </c>
+      <c r="X1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>25</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
         <v>41826</v>
       </c>
@@ -618,7 +630,7 @@
         <v>59</v>
       </c>
       <c r="R2" s="5">
-        <f t="shared" ref="R2:R8" si="1">((P2*3600)+(Q2*60))/E2</f>
+        <f>((P2*3600)+(Q2*60))/E2</f>
         <v>297.61102603369068</v>
       </c>
       <c r="S2" s="5">
@@ -632,20 +644,28 @@
       <c r="U2" s="1">
         <v>0.13040509259259259</v>
       </c>
-      <c r="V2" s="1" t="str">
-        <f t="shared" ref="V2:V13" si="2">TEXT(U2, "hh:mm:ss")</f>
+      <c r="V2" s="5">
+        <f>HOUR(U2)*3600+MINUTE(U2)*60+SECOND(U2)</f>
+        <v>11267</v>
+      </c>
+      <c r="W2" s="5">
+        <f>V2/42.195</f>
+        <v>267.02215902358097</v>
+      </c>
+      <c r="X2" s="1" t="str">
+        <f t="shared" ref="X2:X13" si="1">TEXT(U2, "hh:mm:ss")</f>
         <v>03:07:47</v>
       </c>
-      <c r="W2" s="5" t="str">
-        <f t="shared" ref="W2:W13" si="3">TEXT(ABS(T2 - U2), "mm:ss")</f>
+      <c r="Y2" s="5" t="str">
+        <f t="shared" ref="Y2:Y13" si="2">TEXT(ABS(T2 - U2), "mm:ss")</f>
         <v>03:14</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="Z2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Y2" s="5"/>
+      <c r="AA2" s="5"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>41924</v>
       </c>
@@ -701,7 +721,7 @@
         <v>18</v>
       </c>
       <c r="R3" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="R3:R8" si="3">((P3*3600)+(Q3*60))/E3</f>
         <v>296.74057322648838</v>
       </c>
       <c r="S3" s="5">
@@ -715,19 +735,27 @@
       <c r="U3" s="1">
         <v>0.15145833333333333</v>
       </c>
-      <c r="V3" s="1" t="str">
+      <c r="V3" s="5">
+        <f t="shared" ref="V3:V13" si="4">HOUR(U3)*3600+MINUTE(U3)*60+SECOND(U3)</f>
+        <v>13086</v>
+      </c>
+      <c r="W3" s="5">
+        <f t="shared" ref="W3:W13" si="5">V3/42.195</f>
+        <v>310.13153217205831</v>
+      </c>
+      <c r="X3" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>03:38:06</v>
+      </c>
+      <c r="Y3" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>03:38:06</v>
-      </c>
-      <c r="W3" s="5" t="str">
-        <f t="shared" si="3"/>
         <v>25:35</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Z3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>42114</v>
       </c>
@@ -783,33 +811,41 @@
         <v>31</v>
       </c>
       <c r="R4" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>293.76091757028445</v>
       </c>
       <c r="S4" s="5">
-        <f t="shared" ref="S4:S13" si="4">17.1 + 140 * EXP(-0.0053 * F4) + 0.55 * R4</f>
+        <f t="shared" ref="S4:S13" si="6">17.1 + 140 * EXP(-0.0053 * F4) + 0.55 * R4</f>
         <v>272.32409983009654</v>
       </c>
       <c r="T4" s="5" t="str">
-        <f t="shared" ref="T4:T13" si="5">TEXT((S4 * 42.195)/86400, "hh:mm:ss")</f>
+        <f t="shared" ref="T4:T13" si="7">TEXT((S4 * 42.195)/86400, "hh:mm:ss")</f>
         <v>03:11:31</v>
       </c>
       <c r="U4" s="2">
         <v>0.12847222222222221</v>
       </c>
-      <c r="V4" s="1" t="str">
+      <c r="V4" s="5">
+        <f t="shared" si="4"/>
+        <v>11100</v>
+      </c>
+      <c r="W4" s="5">
+        <f t="shared" si="5"/>
+        <v>263.06434411660149</v>
+      </c>
+      <c r="X4" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>03:05:00</v>
+      </c>
+      <c r="Y4" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>03:05:00</v>
-      </c>
-      <c r="W4" s="5" t="str">
-        <f t="shared" si="3"/>
         <v>06:31</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Z4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>42190</v>
       </c>
@@ -865,33 +901,41 @@
         <v>28</v>
       </c>
       <c r="R5" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>279.68828197612066</v>
       </c>
       <c r="S5" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>267.56799345767769</v>
       </c>
       <c r="T5" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>03:08:10</v>
       </c>
       <c r="U5" s="2">
         <v>0.12375</v>
       </c>
-      <c r="V5" s="1" t="str">
+      <c r="V5" s="5">
+        <f t="shared" si="4"/>
+        <v>10692</v>
+      </c>
+      <c r="W5" s="5">
+        <f t="shared" si="5"/>
+        <v>253.39495200853182</v>
+      </c>
+      <c r="X5" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>02:58:12</v>
+      </c>
+      <c r="Y5" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>02:58:12</v>
-      </c>
-      <c r="W5" s="5" t="str">
-        <f t="shared" si="3"/>
         <v>09:58</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Z5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>42470</v>
       </c>
@@ -909,7 +953,7 @@
         <v>706.19</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F6:F13" si="6">E6/8</f>
+        <f t="shared" ref="F6:F13" si="8">E6/8</f>
         <v>88.273750000000007</v>
       </c>
       <c r="G6" s="1">
@@ -947,33 +991,41 @@
         <v>16</v>
       </c>
       <c r="R6" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>276.63943131451873</v>
       </c>
       <c r="S6" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>256.94025611790721</v>
       </c>
       <c r="T6" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>03:00:42</v>
       </c>
       <c r="U6" s="2">
         <v>0.12593750000000001</v>
       </c>
-      <c r="V6" s="1" t="str">
+      <c r="V6" s="5">
+        <f t="shared" si="4"/>
+        <v>10881</v>
+      </c>
+      <c r="W6" s="5">
+        <f t="shared" si="5"/>
+        <v>257.8741557056523</v>
+      </c>
+      <c r="X6" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>03:01:21</v>
+      </c>
+      <c r="Y6" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>03:01:21</v>
-      </c>
-      <c r="W6" s="5" t="str">
-        <f t="shared" si="3"/>
         <v>00:39</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Z6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>42554</v>
       </c>
@@ -991,7 +1043,7 @@
         <v>452.66999999999996</v>
       </c>
       <c r="F7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>56.583749999999995</v>
       </c>
       <c r="G7" s="1">
@@ -1029,33 +1081,41 @@
         <v>55</v>
       </c>
       <c r="R7" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>317.44979786599515</v>
       </c>
       <c r="S7" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>295.42294701251569</v>
       </c>
       <c r="T7" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>03:27:45</v>
       </c>
       <c r="U7" s="2">
         <v>0.15238425925925925</v>
       </c>
-      <c r="V7" s="1" t="str">
+      <c r="V7" s="5">
+        <f t="shared" si="4"/>
+        <v>13166</v>
+      </c>
+      <c r="W7" s="5">
+        <f t="shared" si="5"/>
+        <v>312.02749140893468</v>
+      </c>
+      <c r="X7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>03:39:26</v>
+      </c>
+      <c r="Y7" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>03:39:26</v>
-      </c>
-      <c r="W7" s="5" t="str">
-        <f t="shared" si="3"/>
         <v>11:41</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Z7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>42680</v>
       </c>
@@ -1073,7 +1133,7 @@
         <v>570.15</v>
       </c>
       <c r="F8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>71.268749999999997</v>
       </c>
       <c r="G8" s="1">
@@ -1111,33 +1171,41 @@
         <v>54</v>
       </c>
       <c r="R8" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>289.81846882399367</v>
       </c>
       <c r="S8" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>272.45887292264371</v>
       </c>
       <c r="T8" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>03:11:36</v>
       </c>
       <c r="U8" s="2">
         <v>0.13693287037037036</v>
       </c>
-      <c r="V8" s="1" t="str">
+      <c r="V8" s="5">
+        <f t="shared" si="4"/>
+        <v>11831</v>
+      </c>
+      <c r="W8" s="5">
+        <f t="shared" si="5"/>
+        <v>280.38867164355969</v>
+      </c>
+      <c r="X8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>03:17:11</v>
+      </c>
+      <c r="Y8" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>03:17:11</v>
-      </c>
-      <c r="W8" s="5" t="str">
-        <f t="shared" si="3"/>
         <v>05:35</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Z8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>43282</v>
       </c>
@@ -1155,7 +1223,7 @@
         <v>707.42</v>
       </c>
       <c r="F9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>88.427499999999995</v>
       </c>
       <c r="G9" s="1">
@@ -1193,33 +1261,41 @@
         <v>41</v>
       </c>
       <c r="R9" s="5">
-        <f t="shared" ref="R9:R13" si="7">((P9*3600)+(Q9*60))/E9</f>
+        <f t="shared" ref="R9:R13" si="9">((P9*3600)+(Q9*60))/E9</f>
         <v>308.812303864748</v>
       </c>
       <c r="S9" s="5">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>274.56390990358597</v>
       </c>
       <c r="T9" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>03:13:05</v>
       </c>
       <c r="U9" s="2">
         <v>0.14848379629629629</v>
       </c>
-      <c r="V9" s="1" t="str">
+      <c r="V9" s="5">
+        <f t="shared" si="4"/>
+        <v>12829</v>
+      </c>
+      <c r="W9" s="5">
+        <f t="shared" si="5"/>
+        <v>304.04076312359285</v>
+      </c>
+      <c r="X9" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>03:33:49</v>
+      </c>
+      <c r="Y9" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>03:33:49</v>
-      </c>
-      <c r="W9" s="5" t="str">
-        <f t="shared" si="3"/>
         <v>20:44</v>
       </c>
-      <c r="X9" t="s">
+      <c r="Z9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>43653</v>
       </c>
@@ -1237,7 +1313,7 @@
         <v>819.5</v>
       </c>
       <c r="F10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>102.4375</v>
       </c>
       <c r="G10" s="1">
@@ -1275,33 +1351,41 @@
         <v>1</v>
       </c>
       <c r="R10" s="5">
+        <f t="shared" si="9"/>
+        <v>290.00610128126908</v>
+      </c>
+      <c r="S10" s="5">
+        <f t="shared" si="6"/>
+        <v>257.95033270898256</v>
+      </c>
+      <c r="T10" s="5" t="str">
         <f t="shared" si="7"/>
-        <v>290.00610128126908</v>
-      </c>
-      <c r="S10" s="5">
-        <f t="shared" si="4"/>
-        <v>257.95033270898256</v>
-      </c>
-      <c r="T10" s="5" t="str">
-        <f t="shared" si="5"/>
         <v>03:01:24</v>
       </c>
       <c r="U10" s="2">
         <v>0.11964120370370371</v>
       </c>
-      <c r="V10" s="1" t="str">
+      <c r="V10" s="5">
+        <f t="shared" si="4"/>
+        <v>10337</v>
+      </c>
+      <c r="W10" s="5">
+        <f t="shared" si="5"/>
+        <v>244.98163289489275</v>
+      </c>
+      <c r="X10" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>02:52:17</v>
+      </c>
+      <c r="Y10" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>02:52:17</v>
-      </c>
-      <c r="W10" s="5" t="str">
-        <f t="shared" si="3"/>
         <v>09:07</v>
       </c>
-      <c r="X10" t="s">
+      <c r="Z10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A11" s="6">
         <v>44745</v>
       </c>
@@ -1319,7 +1403,7 @@
         <v>579.41999999999996</v>
       </c>
       <c r="F11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>72.427499999999995</v>
       </c>
       <c r="G11" s="1">
@@ -1357,33 +1441,41 @@
         <v>44</v>
       </c>
       <c r="R11" s="5">
+        <f t="shared" si="9"/>
+        <v>315.2117634876256</v>
+      </c>
+      <c r="S11" s="5">
+        <f t="shared" si="6"/>
+        <v>285.83767244786816</v>
+      </c>
+      <c r="T11" s="5" t="str">
         <f t="shared" si="7"/>
-        <v>315.2117634876256</v>
-      </c>
-      <c r="S11" s="5">
-        <f t="shared" si="4"/>
-        <v>285.83767244786816</v>
-      </c>
-      <c r="T11" s="5" t="str">
-        <f t="shared" si="5"/>
         <v>03:21:01</v>
       </c>
       <c r="U11" s="2">
         <v>0.12973379629629631</v>
       </c>
-      <c r="V11" s="1" t="str">
+      <c r="V11" s="5">
+        <f t="shared" si="4"/>
+        <v>11209</v>
+      </c>
+      <c r="W11" s="5">
+        <f t="shared" si="5"/>
+        <v>265.64758857684558</v>
+      </c>
+      <c r="X11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>03:06:49</v>
+      </c>
+      <c r="Y11" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>03:06:49</v>
-      </c>
-      <c r="W11" s="5" t="str">
-        <f t="shared" si="3"/>
         <v>14:12</v>
       </c>
-      <c r="X11" t="s">
+      <c r="Z11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A12" s="6">
         <v>45186</v>
       </c>
@@ -1401,7 +1493,7 @@
         <v>638.56000000000006</v>
       </c>
       <c r="F12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>79.820000000000007</v>
       </c>
       <c r="G12" s="1">
@@ -1439,33 +1531,41 @@
         <v>34</v>
       </c>
       <c r="R12" s="5">
+        <f t="shared" si="9"/>
+        <v>318.90503633174637</v>
+      </c>
+      <c r="S12" s="5">
+        <f t="shared" si="6"/>
+        <v>284.20456000874492</v>
+      </c>
+      <c r="T12" s="5" t="str">
         <f t="shared" si="7"/>
-        <v>318.90503633174637</v>
-      </c>
-      <c r="S12" s="5">
-        <f t="shared" si="4"/>
-        <v>284.20456000874492</v>
-      </c>
-      <c r="T12" s="5" t="str">
-        <f t="shared" si="5"/>
         <v>03:19:52</v>
       </c>
       <c r="U12" s="1">
         <v>0.14108796296296297</v>
       </c>
-      <c r="V12" s="1" t="str">
+      <c r="V12" s="5">
+        <f t="shared" si="4"/>
+        <v>12190</v>
+      </c>
+      <c r="W12" s="5">
+        <f t="shared" si="5"/>
+        <v>288.89678871904255</v>
+      </c>
+      <c r="X12" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>03:23:10</v>
+      </c>
+      <c r="Y12" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>03:23:10</v>
-      </c>
-      <c r="W12" s="5" t="str">
-        <f t="shared" si="3"/>
         <v>03:18</v>
       </c>
-      <c r="X12" t="s">
+      <c r="Z12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A13" s="6">
         <v>45480</v>
       </c>
@@ -1483,7 +1583,7 @@
         <v>599.55999999999995</v>
       </c>
       <c r="F13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>74.944999999999993</v>
       </c>
       <c r="G13" s="3">
@@ -1521,33 +1621,42 @@
         <v>32</v>
       </c>
       <c r="R13" s="5">
+        <f t="shared" si="9"/>
+        <v>297.41810661151516</v>
+      </c>
+      <c r="S13" s="5">
+        <f t="shared" si="6"/>
+        <v>274.78709884050608</v>
+      </c>
+      <c r="T13" s="5" t="str">
         <f t="shared" si="7"/>
-        <v>297.41810661151516</v>
-      </c>
-      <c r="S13" s="5">
-        <f t="shared" si="4"/>
-        <v>274.78709884050608</v>
-      </c>
-      <c r="T13" s="5" t="str">
-        <f t="shared" si="5"/>
         <v>03:13:15</v>
       </c>
       <c r="U13" s="1">
         <v>0.1295486111111111</v>
       </c>
-      <c r="V13" s="1" t="str">
+      <c r="V13" s="5">
+        <f t="shared" si="4"/>
+        <v>11193</v>
+      </c>
+      <c r="W13" s="5">
+        <f t="shared" si="5"/>
+        <v>265.26839672947034</v>
+      </c>
+      <c r="X13" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>03:06:33</v>
+      </c>
+      <c r="Y13" s="5" t="str">
         <f t="shared" si="2"/>
-        <v>03:06:33</v>
-      </c>
-      <c r="W13" s="5" t="str">
-        <f t="shared" si="3"/>
         <v>06:42</v>
       </c>
-      <c r="X13" t="s">
+      <c r="Z13" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>